<commit_message>
recent changes have been made
</commit_message>
<xml_diff>
--- a/VeriTabanıTasarımı.xlsx
+++ b/VeriTabanıTasarımı.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ayşegül Ülker\Desktop\Ayşegül_Çalışma\Bilge_Adam_Yazilim_Egitimi\12_School_Automation_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78392149-B056-496D-9ACC-6F1A65A1AECB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD362DC4-5008-462D-98A4-584708C58AA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="149">
   <si>
     <t>OKUL NO</t>
   </si>
@@ -316,12 +316,6 @@
   </si>
   <si>
     <t>FLOOR_LOCATION</t>
-  </si>
-  <si>
-    <t>KAPASİTE</t>
-  </si>
-  <si>
-    <t>CAPACITY</t>
   </si>
   <si>
     <t>DÖNEM BİLGİ TABLOSU</t>
@@ -3707,8 +3701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AD65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9:O19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Q1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AA20" sqref="AA20:AD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -3746,19 +3740,19 @@
   <sheetData>
     <row r="2" spans="2:30" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:30" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
       <c r="G3" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
@@ -3766,44 +3760,44 @@
         <v>56</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
-      <c r="Q3" s="9" t="s">
+      <c r="Q3" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="R3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="V3" s="9" t="s">
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="V3" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="W3" s="9" t="s">
+      <c r="W3" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="X3" s="9"/>
-      <c r="Y3" s="9"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
       <c r="AA3" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AB3" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="AC3" s="10"/>
       <c r="AD3" s="10"/>
     </row>
     <row r="4" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B4" s="9"/>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="10"/>
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="10"/>
@@ -3826,24 +3820,24 @@
       <c r="O4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="3" t="s">
+      <c r="Q4" s="10"/>
+      <c r="R4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="S4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="T4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="V4" s="9"/>
-      <c r="W4" s="3" t="s">
+      <c r="V4" s="10"/>
+      <c r="W4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="X4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="Y4" s="6" t="s">
         <v>7</v>
       </c>
       <c r="AA4" s="10"/>
@@ -3858,16 +3852,16 @@
       </c>
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="8"/>
       <c r="G5" s="7" t="s">
         <v>8</v>
       </c>
@@ -3888,26 +3882,26 @@
         <v>29</v>
       </c>
       <c r="O5" s="7"/>
-      <c r="Q5" s="4" t="s">
+      <c r="Q5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="R5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="S5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="T5" s="4"/>
-      <c r="V5" s="4" t="s">
+      <c r="T5" s="7"/>
+      <c r="V5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="W5" s="4" t="s">
+      <c r="W5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="X5" s="4" t="s">
+      <c r="X5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Y5" s="4"/>
+      <c r="Y5" s="7"/>
       <c r="AA5" s="7" t="s">
         <v>8</v>
       </c>
@@ -3920,21 +3914,21 @@
       <c r="AD5" s="7"/>
     </row>
     <row r="6" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="8"/>
       <c r="G6" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>81</v>
@@ -3950,31 +3944,31 @@
         <v>33</v>
       </c>
       <c r="O6" s="8"/>
-      <c r="Q6" s="4" t="s">
+      <c r="Q6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="R6" s="4" t="s">
+      <c r="R6" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="S6" s="4" t="s">
+      <c r="S6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="T6" s="4"/>
-      <c r="V6" s="4" t="s">
+      <c r="T6" s="7"/>
+      <c r="V6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="W6" s="4" t="s">
+      <c r="W6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="X6" s="4" t="s">
+      <c r="X6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="Y6" s="4"/>
+      <c r="Y6" s="7"/>
       <c r="AA6" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="AB6" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AC6" s="7" t="s">
         <v>33</v>
@@ -3982,105 +3976,105 @@
       <c r="AD6" s="7"/>
     </row>
     <row r="7" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B7" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="B7" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="E7" s="8"/>
       <c r="G7" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>81</v>
       </c>
       <c r="J7" s="8"/>
-      <c r="Q7" s="4" t="s">
+      <c r="Q7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="R7" s="4" t="s">
+      <c r="R7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="S7" s="4" t="s">
+      <c r="S7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="T7" s="4"/>
-      <c r="V7" s="4" t="s">
+      <c r="T7" s="7"/>
+      <c r="V7" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="W7" s="4" t="s">
+      <c r="W7" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="X7" s="4" t="s">
+      <c r="X7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="Y7" s="4"/>
+      <c r="Y7" s="7"/>
     </row>
     <row r="8" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="C8" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="E8" s="8"/>
       <c r="G8" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>72</v>
       </c>
       <c r="J8" s="7"/>
-      <c r="Q8" s="4" t="s">
+      <c r="Q8" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="R8" s="4" t="s">
+      <c r="R8" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="S8" s="4" t="s">
+      <c r="S8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="T8" s="4"/>
-      <c r="V8" s="4" t="s">
+      <c r="T8" s="7"/>
+      <c r="V8" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="W8" s="4" t="s">
+      <c r="W8" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="X8" s="4" t="s">
+      <c r="X8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="Y8" s="4"/>
+      <c r="Y8" s="7"/>
     </row>
     <row r="9" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="8"/>
       <c r="G9" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>72</v>
@@ -4094,46 +4088,46 @@
       </c>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
-      <c r="Q9" s="4" t="s">
+      <c r="Q9" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="R9" s="4" t="s">
+      <c r="R9" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="S9" s="4" t="s">
+      <c r="S9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="T9" s="4"/>
-      <c r="V9" s="4" t="s">
+      <c r="T9" s="7"/>
+      <c r="V9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="W9" s="4" t="s">
+      <c r="W9" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="X9" s="4" t="s">
+      <c r="X9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="Y9" s="4"/>
+      <c r="Y9" s="7"/>
       <c r="AA9" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="AB9" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="AC9" s="9"/>
       <c r="AD9" s="9"/>
     </row>
     <row r="10" spans="2:30" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="5"/>
+      <c r="E10" s="8"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -4148,26 +4142,26 @@
       <c r="O10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="Q10" s="4" t="s">
+      <c r="Q10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="R10" s="4" t="s">
+      <c r="R10" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="S10" s="4" t="s">
+      <c r="S10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="T10" s="5"/>
-      <c r="V10" s="4" t="s">
+      <c r="T10" s="8"/>
+      <c r="V10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="W10" s="4" t="s">
+      <c r="W10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="X10" s="4" t="s">
+      <c r="X10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="Y10" s="4"/>
+      <c r="Y10" s="7"/>
       <c r="AA10" s="9"/>
       <c r="AB10" s="3" t="s">
         <v>5</v>
@@ -4180,16 +4174,16 @@
       </c>
     </row>
     <row r="11" spans="2:30" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="8"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -4205,26 +4199,26 @@
         <v>29</v>
       </c>
       <c r="O11" s="7"/>
-      <c r="Q11" s="4" t="s">
+      <c r="Q11" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="R11" s="4" t="s">
+      <c r="R11" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="S11" s="4" t="s">
+      <c r="S11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="T11" s="5"/>
-      <c r="V11" s="4" t="s">
+      <c r="T11" s="8"/>
+      <c r="V11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="W11" s="4" t="s">
+      <c r="W11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="X11" s="4" t="s">
+      <c r="X11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="Y11" s="4"/>
+      <c r="Y11" s="7"/>
       <c r="AA11" s="4" t="s">
         <v>8</v>
       </c>
@@ -4237,16 +4231,16 @@
       <c r="AD11" s="4"/>
     </row>
     <row r="12" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="5"/>
+      <c r="E12" s="8"/>
       <c r="F12" s="2"/>
       <c r="G12" s="20" t="s">
         <v>41</v>
@@ -4257,42 +4251,42 @@
       <c r="I12" s="18"/>
       <c r="J12" s="19"/>
       <c r="L12" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="N12" s="7" t="s">
         <v>33</v>
       </c>
       <c r="O12" s="8"/>
-      <c r="Q12" s="4" t="s">
+      <c r="Q12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="R12" s="4" t="s">
+      <c r="R12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="S12" s="4" t="s">
+      <c r="S12" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="T12" s="4"/>
-      <c r="V12" s="4" t="s">
+      <c r="T12" s="7"/>
+      <c r="V12" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="W12" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="X12" s="4" t="s">
+      <c r="W12" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="X12" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="Y12" s="5" t="s">
+      <c r="Y12" s="8" t="s">
         <v>36</v>
       </c>
       <c r="AA12" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="AB12" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="AC12" s="4" t="s">
         <v>81</v>
@@ -4300,16 +4294,16 @@
       <c r="AD12" s="4"/>
     </row>
     <row r="13" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="8" t="s">
         <v>36</v>
       </c>
       <c r="F13" s="2"/>
@@ -4324,42 +4318,42 @@
         <v>7</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="N13" s="7" t="s">
         <v>33</v>
       </c>
       <c r="O13" s="8"/>
-      <c r="Q13" s="4" t="s">
+      <c r="Q13" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="R13" s="4" t="s">
+      <c r="R13" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="S13" s="4" t="s">
+      <c r="S13" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="T13" s="4"/>
-      <c r="V13" s="4" t="s">
+      <c r="T13" s="7"/>
+      <c r="V13" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="W13" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="X13" s="4" t="s">
+      <c r="W13" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="X13" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="Y13" s="5" t="s">
+      <c r="Y13" s="8" t="s">
         <v>36</v>
       </c>
       <c r="AA13" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AB13" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AC13" s="4" t="s">
         <v>81</v>
@@ -4367,16 +4361,16 @@
       <c r="AD13" s="4"/>
     </row>
     <row r="14" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="5"/>
+      <c r="E14" s="8"/>
       <c r="F14" s="2"/>
       <c r="G14" s="7" t="s">
         <v>8</v>
@@ -4389,42 +4383,42 @@
       </c>
       <c r="J14" s="7"/>
       <c r="L14" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="N14" s="7" t="s">
         <v>33</v>
       </c>
       <c r="O14" s="8"/>
-      <c r="Q14" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="R14" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="S14" s="4" t="s">
+      <c r="Q14" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="R14" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="S14" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="T14" s="5"/>
-      <c r="V14" s="4" t="s">
+      <c r="T14" s="8"/>
+      <c r="V14" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="W14" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="X14" s="4" t="s">
+      <c r="W14" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="X14" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="Y14" s="5" t="s">
+      <c r="Y14" s="8" t="s">
         <v>36</v>
       </c>
       <c r="AA14" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="AB14" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AC14" s="4" t="s">
         <v>33</v>
@@ -4432,16 +4426,16 @@
       <c r="AD14" s="4"/>
     </row>
     <row r="15" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="8" t="s">
         <v>36</v>
       </c>
       <c r="F15" s="2"/>
@@ -4465,26 +4459,26 @@
         <v>33</v>
       </c>
       <c r="O15" s="8"/>
-      <c r="Q15" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="R15" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="S15" s="4" t="s">
+      <c r="Q15" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="R15" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="S15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="T15" s="5"/>
-      <c r="V15" s="4" t="s">
+      <c r="T15" s="8"/>
+      <c r="V15" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="W15" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="X15" s="4" t="s">
+      <c r="W15" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="X15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Y15" s="5" t="s">
+      <c r="Y15" s="8" t="s">
         <v>36</v>
       </c>
       <c r="AA15" s="4" t="s">
@@ -4499,16 +4493,16 @@
       <c r="AD15" s="4"/>
     </row>
     <row r="16" spans="2:30" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="5"/>
+      <c r="E16" s="8"/>
       <c r="F16" s="2"/>
       <c r="G16" s="7" t="s">
         <v>45</v>
@@ -4532,26 +4526,26 @@
         <v>32</v>
       </c>
       <c r="O16" s="8"/>
-      <c r="Q16" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="R16" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="S16" s="4" t="s">
+      <c r="Q16" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="R16" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="S16" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="T16" s="5"/>
-      <c r="V16" s="4" t="s">
+      <c r="T16" s="8"/>
+      <c r="V16" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="W16" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="X16" s="4" t="s">
+      <c r="W16" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="X16" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="Y16" s="5" t="s">
+      <c r="Y16" s="8" t="s">
         <v>36</v>
       </c>
       <c r="AA16" s="4" t="s">
@@ -4566,24 +4560,24 @@
       <c r="AD16" s="4"/>
     </row>
     <row r="17" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="8" t="s">
         <v>36</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>33</v>
@@ -4599,26 +4593,26 @@
         <v>33</v>
       </c>
       <c r="O17" s="8"/>
-      <c r="Q17" s="4" t="s">
+      <c r="Q17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="R17" s="4" t="s">
+      <c r="R17" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="S17" s="4" t="s">
+      <c r="S17" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="T17" s="5"/>
-      <c r="V17" s="4" t="s">
+      <c r="T17" s="8"/>
+      <c r="V17" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="W17" s="4" t="s">
+      <c r="W17" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="X17" s="4" t="s">
+      <c r="X17" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="Y17" s="5" t="s">
+      <c r="Y17" s="8" t="s">
         <v>36</v>
       </c>
       <c r="AA17" s="4" t="s">
@@ -4633,16 +4627,16 @@
       <c r="AD17" s="4"/>
     </row>
     <row r="18" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="5"/>
+      <c r="E18" s="8"/>
       <c r="F18" s="2"/>
       <c r="G18" s="7" t="s">
         <v>84</v>
@@ -4664,36 +4658,36 @@
         <v>33</v>
       </c>
       <c r="O18" s="8"/>
-      <c r="Q18" s="4" t="s">
+      <c r="Q18" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="R18" s="4" t="s">
+      <c r="R18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="S18" s="4" t="s">
+      <c r="S18" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="T18" s="5" t="s">
+      <c r="T18" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="19" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="5"/>
+      <c r="E19" s="8"/>
       <c r="F19" s="2"/>
       <c r="G19" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I19" s="7" t="s">
         <v>32</v>
@@ -4709,49 +4703,49 @@
         <v>33</v>
       </c>
       <c r="O19" s="8"/>
-      <c r="Q19" s="4" t="s">
+      <c r="Q19" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="R19" s="4" t="s">
+      <c r="R19" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="S19" s="4" t="s">
+      <c r="S19" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="T19" s="5"/>
+      <c r="T19" s="8"/>
     </row>
     <row r="20" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="5"/>
+      <c r="E20" s="8"/>
       <c r="F20" s="2"/>
       <c r="G20" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I20" s="7" t="s">
         <v>32</v>
       </c>
       <c r="J20" s="7"/>
-      <c r="Q20" s="4" t="s">
+      <c r="Q20" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="R20" s="4" t="s">
+      <c r="R20" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="S20" s="4" t="s">
+      <c r="S20" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="T20" s="5" t="s">
+      <c r="T20" s="8" t="s">
         <v>36</v>
       </c>
       <c r="V20" s="9" t="s">
@@ -4763,42 +4757,42 @@
       <c r="X20" s="9"/>
       <c r="Y20" s="9"/>
       <c r="AA20" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="AB20" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="AC20" s="9"/>
       <c r="AD20" s="9"/>
     </row>
     <row r="21" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="5"/>
+      <c r="E21" s="8"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
-      <c r="Q21" s="4" t="s">
+      <c r="Q21" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="R21" s="4" t="s">
+      <c r="R21" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="S21" s="4" t="s">
+      <c r="S21" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="T21" s="5"/>
+      <c r="T21" s="8"/>
       <c r="V21" s="9"/>
       <c r="W21" s="3" t="s">
         <v>5</v>
@@ -4821,16 +4815,16 @@
       </c>
     </row>
     <row r="22" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="8" t="s">
         <v>36</v>
       </c>
       <c r="F22" s="2"/>
@@ -4838,16 +4832,16 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
-      <c r="Q22" s="4" t="s">
+      <c r="Q22" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="R22" s="4" t="s">
+      <c r="R22" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="S22" s="4" t="s">
+      <c r="S22" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="T22" s="5"/>
+      <c r="T22" s="8"/>
       <c r="V22" s="4" t="s">
         <v>8</v>
       </c>
@@ -4879,16 +4873,16 @@
       </c>
       <c r="I23" s="10"/>
       <c r="J23" s="10"/>
-      <c r="Q23" s="4" t="s">
+      <c r="Q23" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="R23" s="4" t="s">
+      <c r="R23" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="S23" s="4" t="s">
+      <c r="S23" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="T23" s="5"/>
+      <c r="T23" s="8"/>
       <c r="V23" s="4" t="s">
         <v>0</v>
       </c>
@@ -4900,10 +4894,10 @@
       </c>
       <c r="Y23" s="4"/>
       <c r="AA23" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="AB23" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="AC23" s="4" t="s">
         <v>29</v>
@@ -4922,16 +4916,16 @@
       <c r="J24" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="Q24" s="4" t="s">
+      <c r="Q24" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="R24" s="4" t="s">
+      <c r="R24" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="S24" s="4" t="s">
+      <c r="S24" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="T24" s="5"/>
+      <c r="T24" s="8"/>
       <c r="V24" s="4" t="s">
         <v>54</v>
       </c>
@@ -4943,10 +4937,10 @@
       </c>
       <c r="Y24" s="4"/>
       <c r="AA24" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AB24" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AC24" s="4" t="s">
         <v>33</v>
@@ -4966,19 +4960,19 @@
       </c>
       <c r="J25" s="7"/>
       <c r="N25" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="O25" s="12"/>
-      <c r="Q25" s="4" t="s">
+      <c r="Q25" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="R25" s="4" t="s">
+      <c r="R25" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="S25" s="4" t="s">
+      <c r="S25" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="T25" s="5" t="s">
+      <c r="T25" s="8" t="s">
         <v>36</v>
       </c>
       <c r="V25" s="4" t="s">
@@ -4992,10 +4986,10 @@
       </c>
       <c r="Y25" s="4"/>
       <c r="AA25" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="AB25" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AC25" s="4" t="s">
         <v>33</v>
@@ -5027,10 +5021,10 @@
       </c>
       <c r="Y26" s="4"/>
       <c r="AA26" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AB26" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="AC26" s="4" t="s">
         <v>32</v>
@@ -5066,10 +5060,10 @@
       </c>
       <c r="Y27" s="4"/>
       <c r="AA27" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="AB27" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="AC27" s="4" t="s">
         <v>34</v>
@@ -5099,14 +5093,14 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
-      <c r="Q29" s="9" t="s">
+      <c r="Q29" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="R29" s="9" t="s">
+      <c r="R29" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="10"/>
       <c r="V29" s="4" t="s">
         <v>74</v>
       </c>
@@ -5123,21 +5117,21 @@
     <row r="30" spans="2:30" x14ac:dyDescent="0.3">
       <c r="F30" s="2"/>
       <c r="G30" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I30" s="10"/>
       <c r="J30" s="10"/>
-      <c r="Q30" s="9"/>
-      <c r="R30" s="3" t="s">
+      <c r="Q30" s="10"/>
+      <c r="R30" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="S30" s="3" t="s">
+      <c r="S30" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="T30" s="3" t="s">
+      <c r="T30" s="6" t="s">
         <v>7</v>
       </c>
       <c r="V30" s="4" t="s">
@@ -5151,23 +5145,23 @@
       </c>
       <c r="Y30" s="4"/>
       <c r="AA30" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AB30" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="AC30" s="9"/>
       <c r="AD30" s="9"/>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
       <c r="F31" s="2"/>
       <c r="G31" s="10"/>
       <c r="H31" s="6" t="s">
@@ -5179,21 +5173,21 @@
       <c r="J31" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="Q31" s="4" t="s">
+      <c r="Q31" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="R31" s="4" t="s">
+      <c r="R31" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="S31" s="4" t="s">
+      <c r="S31" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="T31" s="4"/>
+      <c r="T31" s="7"/>
       <c r="V31" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="W31" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="X31" s="4" t="s">
         <v>81</v>
@@ -5211,14 +5205,14 @@
       </c>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B32" s="9"/>
-      <c r="C32" s="3" t="s">
+      <c r="B32" s="10"/>
+      <c r="C32" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F32" s="2"/>
@@ -5232,16 +5226,16 @@
         <v>29</v>
       </c>
       <c r="J32" s="7"/>
-      <c r="Q32" s="4" t="s">
+      <c r="Q32" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="R32" s="4" t="s">
+      <c r="R32" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="S32" s="4" t="s">
+      <c r="S32" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="T32" s="4"/>
+      <c r="T32" s="7"/>
       <c r="V32" s="4" t="s">
         <v>79</v>
       </c>
@@ -5264,42 +5258,42 @@
       <c r="AD32" s="4"/>
     </row>
     <row r="33" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E33" s="5"/>
+      <c r="E33" s="8"/>
       <c r="F33" s="2"/>
       <c r="G33" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I33" s="7" t="s">
         <v>34</v>
       </c>
       <c r="J33" s="7"/>
-      <c r="Q33" s="4" t="s">
+      <c r="Q33" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="R33" s="4" t="s">
+      <c r="R33" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="S33" s="4" t="s">
+      <c r="S33" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="T33" s="4"/>
+      <c r="T33" s="7"/>
       <c r="V33" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="W33" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="X33" s="4" t="s">
         <v>32</v>
@@ -5317,27 +5311,27 @@
       <c r="AD33" s="4"/>
     </row>
     <row r="34" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B34" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D34" s="4" t="s">
+      <c r="B34" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D34" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E34" s="5"/>
+      <c r="E34" s="8"/>
       <c r="F34" s="2"/>
-      <c r="Q34" s="4" t="s">
+      <c r="Q34" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="R34" s="4" t="s">
+      <c r="R34" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="S34" s="4" t="s">
+      <c r="S34" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="T34" s="4"/>
+      <c r="T34" s="7"/>
       <c r="V34" s="4" t="s">
         <v>82</v>
       </c>
@@ -5360,22 +5354,22 @@
       <c r="AD34" s="5"/>
     </row>
     <row r="35" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E35" s="5"/>
+      <c r="E35" s="8"/>
       <c r="F35" s="2"/>
       <c r="V35" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="W35" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="X35" s="4" t="s">
         <v>29</v>
@@ -5393,40 +5387,40 @@
       <c r="AD35" s="5"/>
     </row>
     <row r="36" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E36" s="5"/>
+      <c r="E36" s="8"/>
       <c r="F36" s="2"/>
       <c r="G36" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I36" s="10"/>
       <c r="J36" s="10"/>
       <c r="V36" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="W36" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="X36" s="4" t="s">
         <v>33</v>
       </c>
       <c r="Y36" s="4"/>
       <c r="AA36" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AB36" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="AC36" s="4" t="s">
         <v>32</v>
@@ -5434,16 +5428,16 @@
       <c r="AD36" s="4"/>
     </row>
     <row r="37" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E37" s="5"/>
+      <c r="E37" s="8"/>
       <c r="F37" s="2"/>
       <c r="G37" s="10"/>
       <c r="H37" s="6" t="s">
@@ -5456,20 +5450,20 @@
         <v>7</v>
       </c>
       <c r="V37" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="W37" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="X37" s="4" t="s">
         <v>33</v>
       </c>
       <c r="Y37" s="4"/>
       <c r="AA37" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="AB37" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="AC37" s="4" t="s">
         <v>34</v>
@@ -5477,16 +5471,6 @@
       <c r="AD37" s="4"/>
     </row>
     <row r="38" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B38" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E38" s="5"/>
       <c r="F38" s="2"/>
       <c r="G38" s="7" t="s">
         <v>8</v>
@@ -5502,10 +5486,10 @@
     <row r="39" spans="2:30" x14ac:dyDescent="0.3">
       <c r="F39" s="2"/>
       <c r="G39" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I39" s="7" t="s">
         <v>32</v>

</xml_diff>